<commit_message>
docs: update project tasks excel with sample data
</commit_message>
<xml_diff>
--- a/project_tasks.xlsx
+++ b/project_tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Security Testing</t>
+          <t>Project Orchestration</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,12 +471,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Red-Teaming Orchestration</t>
+          <t>Red-Teaming Engine</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Core framework for managing adversarial simulations and metrics</t>
+          <t>Core framework for managing adversarial simulations and security metrics</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -498,22 +498,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Security Testing</t>
+          <t>Project Orchestration</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>High-Level</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Vulnerability Scanning</t>
+          <t>RedTeamV2 Orchestrator</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Automated engine for detecting privacy and security leaks in LLM responses</t>
+          <t>Main class for executing test suites and merging multi-modal results</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -540,17 +540,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>High-Level</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Linear Jailbreaking</t>
+          <t>Attack Library</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Iterative intensity scaling for complex jailbreak attempts</t>
+          <t>Collection of diverse adversarial techniques for LLM stress testing</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -560,12 +560,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>In-Progress</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
@@ -582,12 +582,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Crescendo Jailbreaking</t>
+          <t>Linear Jailbreaking</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Multi-turn trust-building attack to bypass safety filters</t>
+          <t>Iterative intensity scaling for complex jailbreak attempts</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bad Likert Judge</t>
+          <t>Crescendo Jailbreaking</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Semantic scoring attack to manipulate subjective LLM evaluations</t>
+          <t>Multi-turn trust-building attack; Sub-tasks: Using Deepteam Library</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
@@ -656,17 +656,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prompt Injection</t>
+          <t>Bad Likert Judge</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Injection of malicious instructions to override system prompts</t>
+          <t>Semantic scoring analysis; Sub-tasks: Using Deepteam Library, Lib changes, Notebook conversion, Integration</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -693,34 +693,34 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Indirect Prompt Injection</t>
+          <t>Prompt Injection</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Testing for vulnerabilities where data contains hidden instructions</t>
+          <t>Direct malicious instruction injection to override safety guardrails</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Adversarial Attacks</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -730,22 +730,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PII Leakage Detection</t>
+          <t>Indirect Prompt Injection</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Identification of sensitive personal data (Email, SSN, Phone) in responses</t>
+          <t>Testing for vulnerabilities where data contains hidden adversarial instructions</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Planned</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -757,22 +757,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>High-Level</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BOLA Detection</t>
+          <t>Detection Framework</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Detecting Broken Object Level Authorization and resource access patterns</t>
+          <t>Specialized checkers for security, privacy, and accuracy leaks</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -782,12 +782,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>In-Progress</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -804,17 +804,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Prompt Leakage Detection</t>
+          <t>PII Leakage Detection</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Identifying extraction of internal system instructions or secret prompts</t>
+          <t>Identification of sensitive personal data (Email, SSN, Phone) in responses</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -841,22 +841,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bias &amp; Fairness Audit</t>
+          <t>BOLA Detection</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Systematic check for demographic bias or unfair demographic skewing</t>
+          <t>Detecting Broken Object Level Authorization and resource access patterns</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -878,12 +878,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Misaccuracy Detection</t>
+          <t>Prompt Leakage Detection</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Detecting hallucinated facts or logically inconsistent responses</t>
+          <t>Identifying extraction of internal system instructions or secret prompts</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -893,34 +893,34 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Platform &amp; UI</t>
+          <t>Vulnerability Checks</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>High-Level</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Streamlit Dashboard</t>
+          <t>Bias &amp; Fairness Audit</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Visual management interface for red-teaming runs and analytics</t>
+          <t>Systematic check for demographic bias or unfair demographic skewing</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -930,19 +930,19 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Planned</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Platform &amp; UI</t>
+          <t>Vulnerability Checks</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -952,27 +952,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Real-time Visualization</t>
+          <t>Misaccuracy Detection</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dynamic progress bars and turn-by-turn result streams</t>
+          <t>Detecting hallucinated facts or logically inconsistent responses</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Planned</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
     </row>
@@ -984,17 +984,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>High-Level</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>JSON Export &amp; History</t>
+          <t>Streamlit UI</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Detailed persistence and historical run comparison views</t>
+          <t>Interactive dashboard for test orchestration and result visualization</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1009,44 +1009,44 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Production Grade</t>
+          <t>Platform &amp; UI</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Roadmap</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Multi-tenant Authentication</t>
+          <t>Historical Analysis</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Enterprise-grade user management and account-level security</t>
+          <t>Detailed comparison of historical runs and JSON result viewers</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1063,27 +1063,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Scalable Task Queues</t>
+          <t>Multi-tenant Auth</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Background processing for high-volume concurrent testing (Redis/Celery)</t>
+          <t>Enterprise-grade user management and account-level security (e.g. Clerk/Auth0)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>High</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -1100,17 +1100,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Enterprise Observability</t>
+          <t>Scalable Task Queues</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Centralized logging and performance monitoring for production uptime</t>
+          <t>Background processing for high-volume concurrent testing using Redis/Celery</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1137,17 +1137,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>API Gateway Security</t>
+          <t>Enterprise Observability</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Secure handling of LLM credentials and encrypted data-at-rest</t>
+          <t>Centralized logging, performance monitoring, and error tracking (Sentry/ELK)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Complex</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -1174,25 +1174,62 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>API Gateway Security</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Secure handling of LLM credentials and encrypted data-at-rest</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Complex</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Production Grade</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Roadmap</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>CI/CD Integration</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Automated security regression tests in the delivery pipeline</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>Planned</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>

</xml_diff>

<commit_message>
docs: upgrade project tasks excel to professional format with sub-tasks
</commit_message>
<xml_diff>
--- a/project_tasks.xlsx
+++ b/project_tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,24 +444,49 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Assigned To</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Estimated Effort</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Sub-Task 1</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Sub-Task 2</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Sub-Task 3</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Sub-Task 4</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Project Orchestration</t>
+          <t>Core Framework</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,34 +496,59 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Red-Teaming Engine</t>
+          <t>Red-Teaming Orchestration Engine</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Core framework for managing adversarial simulations and security metrics</t>
+          <t>Establish the primary execution loop to manage simulation lifecycles and metric aggregation.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Lead Architect</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Implemented</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Complex</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1. Design internal state machine for multi-turn sessions</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2. Implement multi-modal result merging logic</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3. Develop standardized logging interface for attack runners</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>4. Optimize runner initialization for parallel execution</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Project Orchestration</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -508,71 +558,121 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RedTeamV2 Orchestrator</t>
+          <t>Linear Jailbreaking Strategy</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Main class for executing test suites and merging multi-modal results</t>
+          <t>Implement iterative intensity scaling to identify threshold-based security bypasses.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Vineeta</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Implemented</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Medium</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1. Configure jailbreak scoring threshold parameters</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2. Develop turn-based prompt mutation logic</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3. Integrate Deepteam evaluation metrics</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>4. Validate against baseline safety filters</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>High-Level</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Attack Library</t>
+          <t>Crescendo Multi-Turn Attack</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Collection of diverse adversarial techniques for LLM stress testing</t>
+          <t>Simulate progressive trust-building conversation chains to bypass top-level safety layers.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Vineeta</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>In-Progress</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Implemented</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>High</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1. Setup Deepteam library dependencies</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2. Script trust-building interaction sequences</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3. Implement response extraction for next-turn seeding</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>4. Conduct full end-to-end integration testing</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -582,34 +682,59 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Linear Jailbreaking</t>
+          <t>Bad Likert Judge Evaluation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Iterative intensity scaling for complex jailbreak attempts</t>
+          <t>Develop a specialized scoring mechanism to detect subtle semantic harms and bias.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Vineeta</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Implemented</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Medium</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1. Convert experimental notebook code to modular script</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2. Apply required changes to Deepteam library core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3. Implement semantic scoring categorization</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>4. Final review and dashboard integration</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -619,34 +744,59 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Crescendo Jailbreaking</t>
+          <t>Prompt Injection Modules</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Multi-turn trust-building attack; Sub-tasks: Using Deepteam Library</t>
+          <t>Standardize payloads for direct instruction override and system instruction hijacking.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Security Engineer</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Implemented</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>High</t>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1. Curate baseline injection payload library</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2. Implement refusal detection logic</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3. Map successful injections to system instruction sets</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>4. Standardize reporting format for injection success</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -656,34 +806,59 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bad Likert Judge</t>
+          <t>Indirect Prompt Injection Tests</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Semantic scoring analysis; Sub-tasks: Using Deepteam Library, Lib changes, Notebook conversion, Integration</t>
+          <t>Evaluate system vulnerability to adversarial instructions hidden within third-party data.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>Security Intern</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Implemented</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Medium</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1. Research common data-based injection vectors</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2. Implement parser for data-embedded instructions</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>3. Define success criteria for indirect hijacking</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>4. Build playground environment for data testing</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -693,34 +868,59 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Prompt Injection</t>
+          <t>PII Leakage Detection</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Direct malicious instruction injection to override safety guardrails</t>
+          <t>Automate detection of sensitive data leaks including emails, SSNs, and banking info.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Privacy Lead</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Implemented</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Low</t>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1. Implement regex and NER-based PII scanners</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2. Define sensitivity levels for different data types</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3. Map PII hits to specific vulnerability profiles</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>4. Generate auto-mitigation suggestions for developers</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Adversarial Attacks</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -730,27 +930,52 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Indirect Prompt Injection</t>
+          <t>BOLA Authorization Auditing</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Testing for vulnerabilities where data contains hidden adversarial instructions</t>
+          <t>Check for implementation flaws in object-level authorization and unofficial resource access.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Backend Dev</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Implemented</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1. Define resource access pattern baselines</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2. Implement cross-user ID extraction logic</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>3. Validate access tokens against resource ownership</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>4. Report authorization bypass indicators</t>
         </is>
       </c>
     </row>
@@ -762,39 +987,64 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>High-Level</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Detection Framework</t>
+          <t>Prompt Extraction Guardrails</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Specialized checkers for security, privacy, and accuracy leaks</t>
+          <t>Monitor for unauthorized attempts to reveal internal system instructions or API keys.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Lead Engineer</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>In-Progress</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>Implemented</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Medium</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1. Identify keyword-based leakage indicators</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2. Monitor for system message verbatim repetition</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>3. Implement alert system for credential patterns</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>4. Suggest system prompt hardening techniques</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -804,34 +1054,59 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PII Leakage Detection</t>
+          <t>Bias &amp; Fairness Audit Module</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Identification of sensitive personal data (Email, SSN, Phone) in responses</t>
+          <t>Audit LLM responses for demographic skews or unfair stereotypical representations.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1. Define demographic benchmark datasets</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2. Implement persona-based bias testing suites</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>3. Measure statistical skews in response sentiment</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>4. Benchmark against industry fairness standards</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -841,397 +1116,362 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BOLA Detection</t>
+          <t>Misaccuracy &amp; Hallucination Check</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Detecting Broken Object Level Authorization and resource access patterns</t>
+          <t>Identify factually incorrect or logically inconsistent responses during stress tests.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Subject Matter Expert</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>High</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1. Implement cross-referencing with ground truth data</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2. Build logical consistency checkers for long responses</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3. Implement confidence scoring for factual claims</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>4. Flag high-risk hallucinatory patterns</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>Roadmap</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Prompt Leakage Detection</t>
+          <t>Multi-tenant Identity Management</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Identifying extraction of internal system instructions or secret prompts</t>
+          <t>Implement secure user authentication and tenant-level data isolation.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>DevOps Team</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Implemented</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1. Evaluate and integrate Clerk or Auth0</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2. Implement JWT-based RBAC for API endpoints</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>3. Design tenant-isolated database schemas</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>4. Audit session management for security gaps</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>Roadmap</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bias &amp; Fairness Audit</t>
+          <t>Asynchronous Task Queuing</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Systematic check for demographic bias or unfair demographic skewing</t>
+          <t>Transition long-running simulations to background worker processes.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>Backend Team</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>High</t>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1. Configure Redis and Celery worker infrastructure</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2. Implement task status polling endpoints</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3. Handle worker timeout and retry logic</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>4. Optimize database connection pool for concurrent tasks</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Vulnerability Checks</t>
+          <t>Observability</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>Roadmap</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Misaccuracy Detection</t>
+          <t>Enterprise Logging &amp; Monitoring</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Detecting hallucinated facts or logically inconsistent responses</t>
+          <t>Establish centralized monitoring for system health and performance analytics.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>DevOps Lead</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Planned</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>High</t>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1. Configure Sentry for real-time error tracking</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2. Set up ELK stack for centralized log analysis</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3. Develop system health heartbeat monitors</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>4. Implement usage dashboards for resource tracking</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Platform &amp; UI</t>
+          <t>Production Security</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>High-Level</t>
+          <t>Roadmap</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Streamlit UI</t>
+          <t>API Gateway &amp; Secret Management</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Interactive dashboard for test orchestration and result visualization</t>
+          <t>Protect LLM credentials and sensitive user data using enterprise-grade encryption.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>SecOps</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Complex</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1. Implement AWS/Azure Key Vault for API keys</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2. Set up rate limiting and API usage quotas</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3. Implement encryption-at-rest for results database</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>4. Conduct external penetration test on API surface</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Platform &amp; UI</t>
+          <t>CI/CD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Low-Level</t>
+          <t>Roadmap</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Historical Analysis</t>
+          <t>Automated Security Regression</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Detailed comparison of historical runs and JSON result viewers</t>
+          <t>Integrate red-teaming tests directly into the developer deployment workflow.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>Release Engineer</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Implemented</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Production Grade</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Roadmap</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Multi-tenant Auth</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Enterprise-grade user management and account-level security (e.g. Clerk/Auth0)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
           <t>Planned</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Production Grade</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Roadmap</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Scalable Task Queues</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Background processing for high-volume concurrent testing using Redis/Celery</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Production Grade</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Roadmap</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Enterprise Observability</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Centralized logging, performance monitoring, and error tracking (Sentry/ELK)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Production Grade</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Roadmap</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>API Gateway Security</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Secure handling of LLM credentials and encrypted data-at-rest</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Complex</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Production Grade</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Roadmap</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>CI/CD Integration</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Automated security regression tests in the delivery pipeline</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1. Script headless execution of red-teaming suites</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2. Implement pass/fail criteria for PR approvals</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3. Integrate reporting with GitHub Actions</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>4. Automate scheduled full-suite security audits</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: add MongoDB database creation subtasks to project plan
</commit_message>
<xml_diff>
--- a/project_tasks.xlsx
+++ b/project_tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,7 +548,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Security Testing</t>
+          <t>Core Framework</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -558,22 +558,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Linear Jailbreaking Strategy</t>
+          <t>MongoDB Database Architecture</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Implement iterative intensity scaling to identify threshold-based security bypasses.</t>
+          <t>Design and implement a scalable document storage system for red-teaming runs, results, and profiles.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Vineeta</t>
+          <t>Database Engineer</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -588,22 +588,22 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1. Configure jailbreak scoring threshold parameters</t>
+          <t>1. Design and document document schema (Collections for Runs, Results, and Profiles)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2. Develop turn-based prompt mutation logic</t>
+          <t>2. Setup MongoDB environment (Atlas/Local) and configure connection strings</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3. Integrate Deepteam evaluation metrics</t>
+          <t>3. Implement StorageHelper and MongoDBService classes for CRUD operations</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>4. Validate against baseline safety filters</t>
+          <t>4. Develop data migration scripts and validation logic for schema consistency</t>
         </is>
       </c>
     </row>
@@ -620,12 +620,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Crescendo Multi-Turn Attack</t>
+          <t>Linear Jailbreaking Strategy</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Simulate progressive trust-building conversation chains to bypass top-level safety layers.</t>
+          <t>Implement iterative intensity scaling to identify threshold-based security bypasses.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -645,27 +645,27 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1. Setup Deepteam library dependencies</t>
+          <t>1. Configure jailbreak scoring threshold parameters</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2. Script trust-building interaction sequences</t>
+          <t>2. Develop turn-based prompt mutation logic</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>3. Implement response extraction for next-turn seeding</t>
+          <t>3. Integrate Deepteam evaluation metrics</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>4. Conduct full end-to-end integration testing</t>
+          <t>4. Validate against baseline safety filters</t>
         </is>
       </c>
     </row>
@@ -682,12 +682,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bad Likert Judge Evaluation</t>
+          <t>Crescendo Multi-Turn Attack</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Develop a specialized scoring mechanism to detect subtle semantic harms and bias.</t>
+          <t>Simulate progressive trust-building conversation chains to bypass top-level safety layers.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -707,27 +707,27 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1. Convert experimental notebook code to modular script</t>
+          <t>1. Setup Deepteam library dependencies</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2. Apply required changes to Deepteam library core</t>
+          <t>2. Script trust-building interaction sequences</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>3. Implement semantic scoring categorization</t>
+          <t>3. Implement response extraction for next-turn seeding</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>4. Final review and dashboard integration</t>
+          <t>4. Conduct full end-to-end integration testing</t>
         </is>
       </c>
     </row>
@@ -744,22 +744,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Prompt Injection Modules</t>
+          <t>Bad Likert Judge Evaluation</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Standardize payloads for direct instruction override and system instruction hijacking.</t>
+          <t>Develop a specialized scoring mechanism to detect subtle semantic harms and bias.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Security Engineer</t>
+          <t>Vineeta</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -769,27 +769,27 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1. Curate baseline injection payload library</t>
+          <t>1. Convert experimental notebook code to modular script</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2. Implement refusal detection logic</t>
+          <t>2. Apply required changes to Deepteam library core</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>3. Map successful injections to system instruction sets</t>
+          <t>3. Implement semantic scoring categorization</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>4. Standardize reporting format for injection success</t>
+          <t>4. Final review and dashboard integration</t>
         </is>
       </c>
     </row>
@@ -806,59 +806,59 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Indirect Prompt Injection Tests</t>
+          <t>Prompt Injection Modules</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Evaluate system vulnerability to adversarial instructions hidden within third-party data.</t>
+          <t>Standardize payloads for direct instruction override and system instruction hijacking.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Security Intern</t>
+          <t>Security Engineer</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1. Research common data-based injection vectors</t>
+          <t>1. Curate baseline injection payload library</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2. Implement parser for data-embedded instructions</t>
+          <t>2. Implement refusal detection logic</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>3. Define success criteria for indirect hijacking</t>
+          <t>3. Map successful injections to system instruction sets</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>4. Build playground environment for data testing</t>
+          <t>4. Standardize reporting format for injection success</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vulnerability Engine</t>
+          <t>Security Testing</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -868,27 +868,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PII Leakage Detection</t>
+          <t>Indirect Prompt Injection Tests</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Automate detection of sensitive data leaks including emails, SSNs, and banking info.</t>
+          <t>Evaluate system vulnerability to adversarial instructions hidden within third-party data.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Privacy Lead</t>
+          <t>Security Intern</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Implemented</t>
+          <t>Planned</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -898,22 +898,22 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1. Implement regex and NER-based PII scanners</t>
+          <t>1. Research common data-based injection vectors</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2. Define sensitivity levels for different data types</t>
+          <t>2. Implement parser for data-embedded instructions</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>3. Map PII hits to specific vulnerability profiles</t>
+          <t>3. Define success criteria for indirect hijacking</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>4. Generate auto-mitigation suggestions for developers</t>
+          <t>4. Build playground environment for data testing</t>
         </is>
       </c>
     </row>
@@ -930,17 +930,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BOLA Authorization Auditing</t>
+          <t>PII Leakage Detection</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Check for implementation flaws in object-level authorization and unofficial resource access.</t>
+          <t>Automate detection of sensitive data leaks including emails, SSNs, and banking info.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Backend Dev</t>
+          <t>Privacy Lead</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -955,27 +955,27 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1. Define resource access pattern baselines</t>
+          <t>1. Implement regex and NER-based PII scanners</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2. Implement cross-user ID extraction logic</t>
+          <t>2. Define sensitivity levels for different data types</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>3. Validate access tokens against resource ownership</t>
+          <t>3. Map PII hits to specific vulnerability profiles</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>4. Report authorization bypass indicators</t>
+          <t>4. Generate auto-mitigation suggestions for developers</t>
         </is>
       </c>
     </row>
@@ -992,52 +992,52 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Prompt Extraction Guardrails</t>
+          <t>BOLA Authorization Auditing</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Monitor for unauthorized attempts to reveal internal system instructions or API keys.</t>
+          <t>Check for implementation flaws in object-level authorization and unofficial resource access.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Lead Engineer</t>
+          <t>Backend Dev</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Implemented</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Implemented</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1. Identify keyword-based leakage indicators</t>
+          <t>1. Define resource access pattern baselines</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2. Monitor for system message verbatim repetition</t>
+          <t>2. Implement cross-user ID extraction logic</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>3. Implement alert system for credential patterns</t>
+          <t>3. Validate access tokens against resource ownership</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>4. Suggest system prompt hardening techniques</t>
+          <t>4. Report authorization bypass indicators</t>
         </is>
       </c>
     </row>
@@ -1054,52 +1054,52 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bias &amp; Fairness Audit Module</t>
+          <t>Prompt Extraction Guardrails</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Audit LLM responses for demographic skews or unfair stereotypical representations.</t>
+          <t>Monitor for unauthorized attempts to reveal internal system instructions or API keys.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>QA Engineer</t>
+          <t>Lead Engineer</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Implemented</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1. Define demographic benchmark datasets</t>
+          <t>1. Identify keyword-based leakage indicators</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2. Implement persona-based bias testing suites</t>
+          <t>2. Monitor for system message verbatim repetition</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>3. Measure statistical skews in response sentiment</t>
+          <t>3. Implement alert system for credential patterns</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>4. Benchmark against industry fairness standards</t>
+          <t>4. Suggest system prompt hardening techniques</t>
         </is>
       </c>
     </row>
@@ -1116,84 +1116,84 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Misaccuracy &amp; Hallucination Check</t>
+          <t>Bias &amp; Fairness Audit Module</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Identify factually incorrect or logically inconsistent responses during stress tests.</t>
+          <t>Audit LLM responses for demographic skews or unfair stereotypical representations.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Subject Matter Expert</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1. Implement cross-referencing with ground truth data</t>
+          <t>1. Define demographic benchmark datasets</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2. Build logical consistency checkers for long responses</t>
+          <t>2. Implement persona-based bias testing suites</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>3. Implement confidence scoring for factual claims</t>
+          <t>3. Measure statistical skews in response sentiment</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>4. Flag high-risk hallucinatory patterns</t>
+          <t>4. Benchmark against industry fairness standards</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>Vulnerability Engine</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Roadmap</t>
+          <t>Low-Level</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Multi-tenant Identity Management</t>
+          <t>Misaccuracy &amp; Hallucination Check</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Implement secure user authentication and tenant-level data isolation.</t>
+          <t>Identify factually incorrect or logically inconsistent responses during stress tests.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>DevOps Team</t>
+          <t>Subject Matter Expert</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1208,22 +1208,22 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1. Evaluate and integrate Clerk or Auth0</t>
+          <t>1. Implement cross-referencing with ground truth data</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2. Implement JWT-based RBAC for API endpoints</t>
+          <t>2. Build logical consistency checkers for long responses</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>3. Design tenant-isolated database schemas</t>
+          <t>3. Implement confidence scoring for factual claims</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>4. Audit session management for security gaps</t>
+          <t>4. Flag high-risk hallucinatory patterns</t>
         </is>
       </c>
     </row>
@@ -1240,59 +1240,59 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Asynchronous Task Queuing</t>
+          <t>Multi-tenant Identity Management</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Transition long-running simulations to background worker processes.</t>
+          <t>Implement secure user authentication and tenant-level data isolation.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Backend Team</t>
+          <t>DevOps Team</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1. Configure Redis and Celery worker infrastructure</t>
+          <t>1. Evaluate and integrate Clerk or Auth0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2. Implement task status polling endpoints</t>
+          <t>2. Implement JWT-based RBAC for API endpoints</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>3. Handle worker timeout and retry logic</t>
+          <t>3. Design tenant-isolated database schemas</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>4. Optimize database connection pool for concurrent tasks</t>
+          <t>4. Audit session management for security gaps</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Observability</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1302,59 +1302,59 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Enterprise Logging &amp; Monitoring</t>
+          <t>Asynchronous Task Queuing</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Establish centralized monitoring for system health and performance analytics.</t>
+          <t>Transition long-running simulations to background worker processes.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>DevOps Lead</t>
+          <t>Backend Team</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Planned</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1. Configure Sentry for real-time error tracking</t>
+          <t>1. Configure Redis and Celery worker infrastructure</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2. Set up ELK stack for centralized log analysis</t>
+          <t>2. Implement task status polling endpoints</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>3. Develop system health heartbeat monitors</t>
+          <t>3. Handle worker timeout and retry logic</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>4. Implement usage dashboards for resource tracking</t>
+          <t>4. Optimize database connection pool for concurrent tasks</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Production Security</t>
+          <t>Observability</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1364,22 +1364,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>API Gateway &amp; Secret Management</t>
+          <t>Enterprise Logging &amp; Monitoring</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Protect LLM credentials and sensitive user data using enterprise-grade encryption.</t>
+          <t>Establish centralized monitoring for system health and performance analytics.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>SecOps</t>
+          <t>DevOps Lead</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1389,87 +1389,149 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Complex</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1. Implement AWS/Azure Key Vault for API keys</t>
+          <t>1. Configure Sentry for real-time error tracking</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2. Set up rate limiting and API usage quotas</t>
+          <t>2. Set up ELK stack for centralized log analysis</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>3. Implement encryption-at-rest for results database</t>
+          <t>3. Develop system health heartbeat monitors</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>4. Conduct external penetration test on API surface</t>
+          <t>4. Implement usage dashboards for resource tracking</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Production Security</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Roadmap</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>API Gateway &amp; Secret Management</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Protect LLM credentials and sensitive user data using enterprise-grade encryption.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SecOps</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Complex</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1. Implement AWS/Azure Key Vault for API keys</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2. Set up rate limiting and API usage quotas</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3. Implement encryption-at-rest for results database</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>4. Conduct external penetration test on API surface</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>CI/CD</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>Roadmap</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Automated Security Regression</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Integrate red-teaming tests directly into the developer deployment workflow.</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Release Engineer</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Planned</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>1. Script headless execution of red-teaming suites</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>2. Implement pass/fail criteria for PR approvals</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>3. Integrate reporting with GitHub Actions</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>4. Automate scheduled full-suite security audits</t>
         </is>

</xml_diff>